<commit_message>
conditional highlighting, none option
</commit_message>
<xml_diff>
--- a/output/blog_audit.xlsx
+++ b/output/blog_audit.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0.00000"/>
+  </numFmts>
   <fonts count="6">
     <font>
       <name val="Calibri"/>
@@ -156,9 +158,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -166,6 +165,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -677,7 +679,11 @@
       <c r="AS1" s="4" t="n"/>
       <c r="AT1" s="4" t="n"/>
       <c r="AU1" s="4" t="n"/>
-      <c r="AV1" s="4" t="n"/>
+      <c r="AV1" s="5" t="inlineStr">
+        <is>
+          <t>Cost Analysis</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -915,1293 +921,1293 @@
           <t>Bounce Rate</t>
         </is>
       </c>
-      <c r="AV2" s="9" t="inlineStr">
+      <c r="AV2" s="8" t="inlineStr">
         <is>
           <t>API Cost</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>Manufacturing Industry Slow to Adopt Emerging Digital Marketing Software</t>
         </is>
       </c>
-      <c r="B3" s="11" t="inlineStr">
+      <c r="B3" s="10" t="inlineStr">
         <is>
           <t>https://act-on.com/learn/blog/manufacturing-industry-slow-to-adopt-emerging-digital-marketing-software/</t>
         </is>
       </c>
-      <c r="C3" s="10" t="inlineStr">
+      <c r="C3" s="9" t="inlineStr">
         <is>
           <t>manufacturing-industry-slow-to-adopt-emerging-digital-marketing-software</t>
         </is>
       </c>
-      <c r="D3" s="10" t="inlineStr">
+      <c r="D3" s="9" t="inlineStr">
         <is>
           <t>2019-05-28</t>
         </is>
       </c>
-      <c r="E3" s="10" t="inlineStr">
+      <c r="E3" s="9" t="inlineStr">
         <is>
           <t>2020-08-14</t>
         </is>
       </c>
-      <c r="F3" s="10" t="n">
+      <c r="F3" s="9" t="n">
         <v>1053</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="G3" s="9" t="n">
         <v>16.1</v>
       </c>
-      <c r="H3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="M3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="N3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="O3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="P3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Q3" s="10" t="inlineStr">
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="M3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="O3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="P3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Q3" s="9" t="inlineStr">
         <is>
           <t>Marketing Automation for Manufacturing</t>
         </is>
       </c>
-      <c r="R3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="S3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="T3" s="10" t="inlineStr">
+      <c r="R3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="S3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="T3" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="U3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="V3" s="10" t="inlineStr">
+      <c r="U3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="V3" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W3" s="10" t="n">
+      <c r="W3" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="X3" s="10" t="n">
+      <c r="X3" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="Y3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Z3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AA3" s="10" t="n">
+      <c r="Y3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Z3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AA3" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="AB3" s="12" t="n">
+      <c r="AB3" s="11" t="n">
         <v>351</v>
       </c>
-      <c r="AC3" s="10" t="n">
+      <c r="AC3" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="AD3" s="10" t="inlineStr">
+      <c r="AD3" s="9" t="inlineStr">
         <is>
           <t>https://act-on.com/wp-content/uploads/2020/06/MA-for-Manufacturing-Feature.jpg</t>
         </is>
       </c>
-      <c r="AE3" s="10" t="inlineStr">
+      <c r="AE3" s="9" t="inlineStr">
         <is>
           <t>Marketing Automation Adoption in Manufacturing Stats</t>
         </is>
       </c>
-      <c r="AF3" s="10" t="n">
+      <c r="AF3" s="9" t="n">
         <v>1024</v>
       </c>
-      <c r="AG3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AH3" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AI3" s="10" t="inlineStr">
+      <c r="AG3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AH3" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AI3" s="9" t="inlineStr">
         <is>
           <t>Industry</t>
         </is>
       </c>
-      <c r="AJ3" s="10" t="inlineStr">
+      <c r="AJ3" s="9" t="inlineStr">
         <is>
           <t>Personalize Outreach and Communication</t>
         </is>
       </c>
-      <c r="AK3" s="10" t="inlineStr">
-        <is>
-          <t>Nurture Prospects</t>
-        </is>
-      </c>
-      <c r="AL3" s="10" t="inlineStr">
+      <c r="AK3" s="9" t="inlineStr">
+        <is>
+          <t>Personalize Outreach</t>
+        </is>
+      </c>
+      <c r="AL3" s="9" t="inlineStr">
         <is>
           <t>GET</t>
         </is>
       </c>
-      <c r="AM3" s="10" t="inlineStr">
+      <c r="AM3" s="9" t="inlineStr">
         <is>
           <t>Build Pipeline and Accelerate Sales</t>
         </is>
       </c>
-      <c r="AN3" s="10" t="inlineStr">
+      <c r="AN3" s="9" t="inlineStr">
         <is>
           <t>Marketing Automation</t>
         </is>
       </c>
-      <c r="AO3" s="10" t="inlineStr">
+      <c r="AO3" s="9" t="inlineStr">
         <is>
           <t>Marketing Leaders</t>
         </is>
       </c>
-      <c r="AP3" s="10" t="n">
+      <c r="AP3" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="AQ3" s="10" t="n">
+      <c r="AQ3" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="AR3" s="10" t="n">
+      <c r="AR3" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="AS3" s="10" t="n">
+      <c r="AS3" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AT3" s="10" t="n">
+      <c r="AT3" s="9" t="n">
         <v>159.51</v>
       </c>
-      <c r="AU3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="10" t="inlineStr">
-        <is>
-          <t>$0.0083</t>
+      <c r="AU3" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="12" t="inlineStr">
+        <is>
+          <t>$0.0088</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="inlineStr">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>Retention Marketing: How We Reached 400 Customer Accounts with a Refreshed Program</t>
         </is>
       </c>
-      <c r="B4" s="11" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>https://act-on.com/learn/blog/retention-marketing-how-we-reached-400-customer-accounts/</t>
         </is>
       </c>
-      <c r="C4" s="10" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
           <t>retention-marketing-how-we-reached-400-customer-accounts</t>
         </is>
       </c>
-      <c r="D4" s="10" t="inlineStr">
+      <c r="D4" s="9" t="inlineStr">
         <is>
           <t>2024-05-07</t>
         </is>
       </c>
-      <c r="E4" s="10" t="inlineStr">
+      <c r="E4" s="9" t="inlineStr">
         <is>
           <t>2024-05-07</t>
         </is>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F4" s="9" t="n">
         <v>1035</v>
       </c>
-      <c r="G4" s="10" t="n">
+      <c r="G4" s="9" t="n">
         <v>9.300000000000001</v>
       </c>
-      <c r="H4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="M4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="N4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="O4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="P4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Q4" s="10" t="inlineStr">
+      <c r="H4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="M4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="O4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="P4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Q4" s="9" t="inlineStr">
         <is>
           <t>retention marketing</t>
         </is>
       </c>
-      <c r="R4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="S4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="T4" s="10" t="inlineStr">
+      <c r="R4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="S4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="T4" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="U4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="V4" s="10" t="inlineStr">
+      <c r="U4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="V4" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W4" s="10" t="n">
+      <c r="W4" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="X4" s="10" t="n">
+      <c r="X4" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="Y4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Z4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AA4" s="10" t="n">
+      <c r="Y4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Z4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AA4" s="9" t="n">
         <v>4</v>
       </c>
       <c r="AB4" s="13" t="n">
         <v>1200</v>
       </c>
-      <c r="AC4" s="10" t="n">
+      <c r="AC4" s="9" t="n">
         <v>628</v>
       </c>
-      <c r="AD4" s="10" t="inlineStr">
+      <c r="AD4" s="9" t="inlineStr">
         <is>
           <t>https://act-on.com/wp-content/uploads/2024/05/retention-marketing-h.jpg</t>
         </is>
       </c>
-      <c r="AE4" s="10" t="inlineStr">
+      <c r="AE4" s="9" t="inlineStr">
         <is>
           <t>two business people shake hands to illustrate retention marketing</t>
         </is>
       </c>
-      <c r="AF4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AH4" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AI4" s="10" t="inlineStr">
+      <c r="AF4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AH4" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AI4" s="9" t="inlineStr">
         <is>
           <t>Use Case</t>
         </is>
       </c>
-      <c r="AJ4" s="10" t="inlineStr">
+      <c r="AJ4" s="9" t="inlineStr">
         <is>
           <t>Personalize Outreach and Communication</t>
         </is>
       </c>
-      <c r="AK4" s="10" t="inlineStr">
-        <is>
-          <t>Nurture Customers</t>
-        </is>
-      </c>
-      <c r="AL4" s="10" t="inlineStr">
-        <is>
-          <t>KEEP</t>
-        </is>
-      </c>
-      <c r="AM4" s="10" t="inlineStr">
-        <is>
-          <t>Deliver Value and Keep Customers</t>
-        </is>
-      </c>
-      <c r="AN4" s="10" t="inlineStr">
+      <c r="AK4" s="9" t="inlineStr">
+        <is>
+          <t>Grow Advocates</t>
+        </is>
+      </c>
+      <c r="AL4" s="9" t="inlineStr">
+        <is>
+          <t>GROW</t>
+        </is>
+      </c>
+      <c r="AM4" s="9" t="inlineStr">
+        <is>
+          <t>Improve Brand Loyalty</t>
+        </is>
+      </c>
+      <c r="AN4" s="9" t="inlineStr">
         <is>
           <t>Customer Marketing</t>
         </is>
       </c>
-      <c r="AO4" s="10" t="inlineStr">
+      <c r="AO4" s="9" t="inlineStr">
         <is>
           <t>Marketing Leaders</t>
         </is>
       </c>
-      <c r="AP4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="10" t="inlineStr">
-        <is>
-          <t>$0.0084</t>
+      <c r="AP4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="12" t="inlineStr">
+        <is>
+          <t>$0.0088</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>How to Calculate Customer Lifetime Value for B2B Marketing</t>
         </is>
       </c>
-      <c r="B5" s="11" t="inlineStr">
+      <c r="B5" s="10" t="inlineStr">
         <is>
           <t>https://act-on.com/learn/blog/how-and-why-you-should-calculate-customer-lifetime-value-clv/</t>
         </is>
       </c>
-      <c r="C5" s="10" t="inlineStr">
+      <c r="C5" s="9" t="inlineStr">
         <is>
           <t>how-and-why-you-should-calculate-customer-lifetime-value-clv</t>
         </is>
       </c>
-      <c r="D5" s="10" t="inlineStr">
+      <c r="D5" s="9" t="inlineStr">
         <is>
           <t>2023-08-01</t>
         </is>
       </c>
-      <c r="E5" s="10" t="inlineStr">
+      <c r="E5" s="9" t="inlineStr">
         <is>
           <t>2024-11-13</t>
         </is>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="9" t="n">
         <v>1171</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="G5" s="9" t="n">
         <v>11.3</v>
       </c>
-      <c r="H5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="M5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="N5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="O5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="P5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Q5" s="10" t="inlineStr">
+      <c r="H5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="M5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="O5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="P5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Q5" s="9" t="inlineStr">
         <is>
           <t>how to calculate customer lifetime value</t>
         </is>
       </c>
-      <c r="R5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="S5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="T5" s="10" t="inlineStr">
+      <c r="R5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="S5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="T5" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="U5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="V5" s="10" t="inlineStr">
+      <c r="U5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="V5" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W5" s="10" t="n">
+      <c r="W5" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="X5" s="10" t="n">
+      <c r="X5" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="Y5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Z5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AA5" s="10" t="n">
+      <c r="Y5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Z5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AA5" s="9" t="n">
         <v>4</v>
       </c>
       <c r="AB5" s="13" t="n">
         <v>1200</v>
       </c>
-      <c r="AC5" s="10" t="n">
+      <c r="AC5" s="9" t="n">
         <v>628</v>
       </c>
-      <c r="AD5" s="10" t="inlineStr">
+      <c r="AD5" s="9" t="inlineStr">
         <is>
           <t>https://act-on.com/wp-content/uploads/2023/08/Shutterstock_2190096895.jpg</t>
         </is>
       </c>
-      <c r="AE5" s="10" t="inlineStr">
+      <c r="AE5" s="9" t="inlineStr">
         <is>
           <t>closeup of hands interacting with marketing metrics like customer lifetime value on a tablet</t>
         </is>
       </c>
-      <c r="AF5" s="10" t="n">
+      <c r="AF5" s="9" t="n">
         <v>1024</v>
       </c>
-      <c r="AG5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AH5" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AI5" s="10" t="inlineStr">
-        <is>
-          <t>Use Case</t>
-        </is>
-      </c>
-      <c r="AJ5" s="10" t="inlineStr">
+      <c r="AG5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AH5" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AI5" s="9" t="inlineStr">
+        <is>
+          <t>Thought Leadership</t>
+        </is>
+      </c>
+      <c r="AJ5" s="9" t="inlineStr">
         <is>
           <t>Personalize Outreach and Communication</t>
         </is>
       </c>
-      <c r="AK5" s="10" t="inlineStr">
+      <c r="AK5" s="9" t="inlineStr">
         <is>
           <t>Cross-sell and Upsell</t>
         </is>
       </c>
-      <c r="AL5" s="10" t="inlineStr">
+      <c r="AL5" s="9" t="inlineStr">
         <is>
           <t>GROW</t>
         </is>
       </c>
-      <c r="AM5" s="10" t="inlineStr">
-        <is>
-          <t>Maximize ARPU</t>
-        </is>
-      </c>
-      <c r="AN5" s="10" t="inlineStr">
-        <is>
-          <t>Marketing Automation</t>
-        </is>
-      </c>
-      <c r="AO5" s="10" t="inlineStr">
+      <c r="AM5" s="9" t="inlineStr">
+        <is>
+          <t>Improve Brand Loyalty</t>
+        </is>
+      </c>
+      <c r="AN5" s="9" t="inlineStr">
+        <is>
+          <t>Customer Marketing</t>
+        </is>
+      </c>
+      <c r="AO5" s="9" t="inlineStr">
         <is>
           <t>Marketing Leaders</t>
         </is>
       </c>
-      <c r="AP5" s="10" t="n">
+      <c r="AP5" s="9" t="n">
         <v>27</v>
       </c>
-      <c r="AQ5" s="10" t="n">
+      <c r="AQ5" s="9" t="n">
         <v>15</v>
       </c>
-      <c r="AR5" s="10" t="n">
+      <c r="AR5" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="AS5" s="10" t="n">
+      <c r="AS5" s="9" t="n">
         <v>0.8182</v>
       </c>
-      <c r="AT5" s="10" t="n">
+      <c r="AT5" s="9" t="n">
         <v>116.8</v>
       </c>
-      <c r="AU5" s="10" t="n">
+      <c r="AU5" s="9" t="n">
         <v>0.1818</v>
       </c>
-      <c r="AV5" s="10" t="inlineStr">
-        <is>
-          <t>$0.0088</t>
+      <c r="AV5" s="12" t="inlineStr">
+        <is>
+          <t>$0.0093</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>Customer Acquisition: Face Economic Headwinds and Win</t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>https://act-on.com/learn/blog/pipeline-generation-face-economic-headwinds-and-win/</t>
         </is>
       </c>
-      <c r="C6" s="10" t="inlineStr">
+      <c r="C6" s="9" t="inlineStr">
         <is>
           <t>pipeline-generation-face-economic-headwinds-and-win</t>
         </is>
       </c>
-      <c r="D6" s="10" t="inlineStr">
+      <c r="D6" s="9" t="inlineStr">
         <is>
           <t>2024-03-19</t>
         </is>
       </c>
-      <c r="E6" s="10" t="inlineStr">
+      <c r="E6" s="9" t="inlineStr">
         <is>
           <t>2024-04-29</t>
         </is>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="F6" s="9" t="n">
         <v>1028</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="9" t="n">
         <v>11.2</v>
       </c>
-      <c r="H6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="M6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="N6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="O6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="P6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Q6" s="10" t="inlineStr">
+      <c r="H6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="M6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="O6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="P6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Q6" s="9" t="inlineStr">
         <is>
           <t>pipeline marketing</t>
         </is>
       </c>
-      <c r="R6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="S6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="T6" s="10" t="inlineStr">
+      <c r="R6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="S6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="T6" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="U6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="V6" s="10" t="inlineStr">
+      <c r="U6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="V6" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W6" s="10" t="n">
+      <c r="W6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="X6" s="10" t="n">
+      <c r="X6" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="Y6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Z6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AA6" s="10" t="n">
+      <c r="Y6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Z6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AA6" s="9" t="n">
         <v>3</v>
       </c>
       <c r="AB6" s="13" t="n">
         <v>1200</v>
       </c>
-      <c r="AC6" s="10" t="n">
+      <c r="AC6" s="9" t="n">
         <v>628</v>
       </c>
-      <c r="AD6" s="10" t="inlineStr">
+      <c r="AD6" s="9" t="inlineStr">
         <is>
           <t>https://act-on.com/wp-content/uploads/2024/03/pipeline-generationh.jpg</t>
         </is>
       </c>
-      <c r="AE6" s="10" t="inlineStr">
+      <c r="AE6" s="9" t="inlineStr">
         <is>
           <t>an executive in a suit represented in black and white, outlined in brand colors</t>
         </is>
       </c>
-      <c r="AF6" s="10" t="n">
+      <c r="AF6" s="9" t="n">
         <v>1024</v>
       </c>
-      <c r="AG6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AH6" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AI6" s="10" t="inlineStr">
+      <c r="AG6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AH6" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AI6" s="9" t="inlineStr">
         <is>
           <t>Industry</t>
         </is>
       </c>
-      <c r="AJ6" s="10" t="inlineStr">
-        <is>
-          <t>Scale Demand Generation Operations</t>
-        </is>
-      </c>
-      <c r="AK6" s="10" t="inlineStr">
-        <is>
-          <t>Deliver Leads</t>
-        </is>
-      </c>
-      <c r="AL6" s="10" t="inlineStr">
+      <c r="AJ6" s="9" t="inlineStr">
+        <is>
+          <t>Personalize Outreach and Communication</t>
+        </is>
+      </c>
+      <c r="AK6" s="9" t="inlineStr">
+        <is>
+          <t>Nurture Prospects</t>
+        </is>
+      </c>
+      <c r="AL6" s="9" t="inlineStr">
         <is>
           <t>GET</t>
         </is>
       </c>
-      <c r="AM6" s="10" t="inlineStr">
+      <c r="AM6" s="9" t="inlineStr">
         <is>
           <t>Build Pipeline and Accelerate Sales</t>
         </is>
       </c>
-      <c r="AN6" s="10" t="inlineStr">
+      <c r="AN6" s="9" t="inlineStr">
         <is>
           <t>Marketing Automation</t>
         </is>
       </c>
-      <c r="AO6" s="10" t="inlineStr">
+      <c r="AO6" s="9" t="inlineStr">
         <is>
           <t>Marketing Leaders</t>
         </is>
       </c>
-      <c r="AP6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="10" t="inlineStr">
-        <is>
-          <t>$0.0083</t>
+      <c r="AP6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="12" t="inlineStr">
+        <is>
+          <t>$0.0089</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="10" t="inlineStr">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>What Is Customer Marketing?</t>
         </is>
       </c>
-      <c r="B7" s="11" t="inlineStr">
+      <c r="B7" s="10" t="inlineStr">
         <is>
           <t>https://act-on.com/learn/blog/what-is-customer-marketing-2/</t>
         </is>
       </c>
-      <c r="C7" s="10" t="inlineStr">
+      <c r="C7" s="9" t="inlineStr">
         <is>
           <t>what-is-customer-marketing-2</t>
         </is>
       </c>
-      <c r="D7" s="10" t="inlineStr">
+      <c r="D7" s="9" t="inlineStr">
         <is>
           <t>2024-05-29</t>
         </is>
       </c>
-      <c r="E7" s="10" t="inlineStr">
+      <c r="E7" s="9" t="inlineStr">
         <is>
           <t>2024-05-29</t>
         </is>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="9" t="n">
         <v>1214</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="G7" s="9" t="n">
         <v>8.1</v>
       </c>
-      <c r="H7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="M7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="N7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="O7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="P7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Q7" s="10" t="inlineStr">
+      <c r="H7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="M7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="O7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="P7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Q7" s="9" t="inlineStr">
         <is>
           <t>customer marketing</t>
         </is>
       </c>
-      <c r="R7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="S7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="T7" s="10" t="inlineStr">
+      <c r="R7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="S7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="T7" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="U7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="V7" s="10" t="inlineStr">
+      <c r="U7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="V7" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W7" s="10" t="n">
+      <c r="W7" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="X7" s="10" t="n">
+      <c r="X7" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="Y7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Z7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AA7" s="10" t="n">
+      <c r="Y7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Z7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AA7" s="9" t="n">
         <v>2</v>
       </c>
       <c r="AB7" s="13" t="n">
         <v>1200</v>
       </c>
-      <c r="AC7" s="10" t="n">
+      <c r="AC7" s="9" t="n">
         <v>628</v>
       </c>
-      <c r="AD7" s="10" t="inlineStr">
+      <c r="AD7" s="9" t="inlineStr">
         <is>
           <t>https://act-on.com/wp-content/uploads/2024/05/customer-marketing-header.jpg</t>
         </is>
       </c>
-      <c r="AE7" s="10" t="inlineStr">
+      <c r="AE7" s="9" t="inlineStr">
         <is>
           <t>customer marketing</t>
         </is>
       </c>
-      <c r="AF7" s="10" t="n">
+      <c r="AF7" s="9" t="n">
         <v>1024</v>
       </c>
-      <c r="AG7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AH7" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AI7" s="10" t="inlineStr">
-        <is>
-          <t>Thought Leadership</t>
-        </is>
-      </c>
-      <c r="AJ7" s="10" t="inlineStr">
+      <c r="AG7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AH7" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AI7" s="9" t="inlineStr">
+        <is>
+          <t>Use Case</t>
+        </is>
+      </c>
+      <c r="AJ7" s="9" t="inlineStr">
         <is>
           <t>Personalize Outreach and Communication</t>
         </is>
       </c>
-      <c r="AK7" s="10" t="inlineStr">
-        <is>
-          <t>Nurture Customers</t>
-        </is>
-      </c>
-      <c r="AL7" s="10" t="inlineStr">
-        <is>
-          <t>KEEP</t>
-        </is>
-      </c>
-      <c r="AM7" s="10" t="inlineStr">
-        <is>
-          <t>Deliver Value and Keep Customers</t>
-        </is>
-      </c>
-      <c r="AN7" s="10" t="inlineStr">
+      <c r="AK7" s="9" t="inlineStr">
+        <is>
+          <t>Cross-sell and Upsell</t>
+        </is>
+      </c>
+      <c r="AL7" s="9" t="inlineStr">
+        <is>
+          <t>GROW</t>
+        </is>
+      </c>
+      <c r="AM7" s="9" t="inlineStr">
+        <is>
+          <t>Improve Brand Loyalty</t>
+        </is>
+      </c>
+      <c r="AN7" s="9" t="inlineStr">
         <is>
           <t>Customer Marketing</t>
         </is>
       </c>
-      <c r="AO7" s="10" t="inlineStr">
+      <c r="AO7" s="9" t="inlineStr">
         <is>
           <t>Marketing Leaders</t>
         </is>
       </c>
-      <c r="AP7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV7" s="10" t="inlineStr">
-        <is>
-          <t>$0.0091</t>
+      <c r="AP7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="12" t="inlineStr">
+        <is>
+          <t>$0.0096</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="inlineStr">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>Act-On Advanced CRM Mapping</t>
         </is>
       </c>
-      <c r="B8" s="11" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>https://act-on.com/learn/data-sheets/advanced-crm-mapping/</t>
         </is>
       </c>
-      <c r="C8" s="10" t="inlineStr">
+      <c r="C8" s="9" t="inlineStr">
         <is>
           <t>advanced-crm-mapping</t>
         </is>
       </c>
-      <c r="D8" s="10" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
         <is>
           <t>2024-08-27</t>
         </is>
       </c>
-      <c r="E8" s="10" t="inlineStr">
+      <c r="E8" s="9" t="inlineStr">
         <is>
           <t>2024-09-05</t>
         </is>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="G8" s="9" t="n">
         <v>25.3</v>
       </c>
-      <c r="H8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="I8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="J8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="K8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="L8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="M8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="N8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="O8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="P8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Q8" s="10" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="I8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="J8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="K8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="L8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="M8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="N8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="O8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="P8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Q8" s="9" t="inlineStr">
         <is>
           <t>Not Found</t>
         </is>
       </c>
-      <c r="R8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="S8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="T8" s="10" t="inlineStr">
+      <c r="R8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="S8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="T8" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="U8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="V8" s="10" t="inlineStr">
+      <c r="U8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="V8" s="9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="W8" s="10" t="n">
+      <c r="W8" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="X8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="Z8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AA8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="10" t="inlineStr">
+      <c r="X8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="Z8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AA8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="9" t="inlineStr">
         <is>
           <t>No Source</t>
         </is>
       </c>
-      <c r="AE8" s="10" t="inlineStr">
+      <c r="AE8" s="9" t="inlineStr">
         <is>
           <t>No Alt Text</t>
         </is>
       </c>
-      <c r="AF8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AH8" s="10" t="inlineStr">
-        <is>
-          <t>TBD</t>
-        </is>
-      </c>
-      <c r="AI8" s="10" t="inlineStr">
+      <c r="AF8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AH8" s="9" t="inlineStr">
+        <is>
+          <t>TBD</t>
+        </is>
+      </c>
+      <c r="AI8" s="9" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="AJ8" s="10" t="inlineStr">
-        <is>
-          <t>Identify and Target Audience Segments</t>
-        </is>
-      </c>
-      <c r="AK8" s="10" t="inlineStr">
-        <is>
-          <t>Segment Audiences</t>
-        </is>
-      </c>
-      <c r="AL8" s="10" t="inlineStr">
+      <c r="AJ8" s="9" t="inlineStr">
+        <is>
+          <t>Personalize Outreach and Communication</t>
+        </is>
+      </c>
+      <c r="AK8" s="9" t="inlineStr">
+        <is>
+          <t>Personalize Outreach</t>
+        </is>
+      </c>
+      <c r="AL8" s="9" t="inlineStr">
         <is>
           <t>GET</t>
         </is>
       </c>
-      <c r="AM8" s="10" t="inlineStr">
+      <c r="AM8" s="9" t="inlineStr">
         <is>
           <t>New Customer Acquisition</t>
         </is>
       </c>
-      <c r="AN8" s="10" t="inlineStr">
+      <c r="AN8" s="9" t="inlineStr">
         <is>
           <t>Marketing Automation</t>
         </is>
       </c>
-      <c r="AO8" s="10" t="inlineStr">
+      <c r="AO8" s="9" t="inlineStr">
         <is>
           <t>Marketing Operations Managers</t>
         </is>
       </c>
-      <c r="AP8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="10" t="inlineStr">
-        <is>
-          <t>$0.0044</t>
+      <c r="AP8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="12" t="inlineStr">
+        <is>
+          <t>$0.0049</t>
         </is>
       </c>
     </row>

</xml_diff>